<commit_message>
before merging with danwadaag
</commit_message>
<xml_diff>
--- a/docs/ewea/ewea communities districts and fms.xlsx
+++ b/docs/ewea/ewea communities districts and fms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs Developement\rstudio\Testing\core\docs\ewea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98848861-8C97-47C3-A63B-58F1385C74E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC878CE9-1DC1-4CF0-80DE-0907047C75FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0052D8CE-578C-4384-ABBC-B6D3FDE38954}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="231">
   <si>
     <t>FMS</t>
   </si>
@@ -452,9 +452,6 @@
     <t>Bandarqaali</t>
   </si>
   <si>
-    <t>Galkacyo</t>
-  </si>
-  <si>
     <t>Bitaale</t>
   </si>
   <si>
@@ -729,6 +726,12 @@
   </si>
   <si>
     <t>Community_name</t>
+  </si>
+  <si>
+    <t>Galkacyo-North</t>
+  </si>
+  <si>
+    <t>Galkacyo-South</t>
   </si>
 </sst>
 </file>
@@ -1135,20 +1138,20 @@
   <dimension ref="A1:F183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F116" sqref="F116"/>
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>34</v>
@@ -1168,7 +1171,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1188,7 +1191,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1208,7 +1211,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1308,7 +1311,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1328,7 +1331,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1348,7 +1351,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1368,7 +1371,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1388,7 +1391,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -1428,7 +1431,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1468,7 +1471,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1488,7 +1491,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -1508,7 +1511,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1528,7 +1531,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -1548,7 +1551,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1608,7 +1611,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -1648,7 +1651,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1668,7 +1671,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -1708,7 +1711,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -1768,7 +1771,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
@@ -1788,7 +1791,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
@@ -1808,7 +1811,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
@@ -1828,7 +1831,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -1848,7 +1851,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
@@ -1868,7 +1871,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -1888,7 +1891,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
@@ -1908,7 +1911,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -1928,7 +1931,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -1948,7 +1951,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
@@ -1988,7 +1991,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
@@ -2008,7 +2011,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
@@ -2028,7 +2031,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
@@ -2068,7 +2071,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
@@ -2088,7 +2091,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
@@ -2108,7 +2111,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -2128,7 +2131,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -2148,7 +2151,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
@@ -2168,7 +2171,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>2</v>
       </c>
@@ -2188,7 +2191,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>2</v>
       </c>
@@ -2208,7 +2211,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>2</v>
       </c>
@@ -2228,7 +2231,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>2</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>2</v>
       </c>
@@ -2268,7 +2271,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>2</v>
       </c>
@@ -2288,7 +2291,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>2</v>
       </c>
@@ -2308,7 +2311,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>2</v>
       </c>
@@ -2328,7 +2331,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>2</v>
       </c>
@@ -2348,7 +2351,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
@@ -2368,7 +2371,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>2</v>
       </c>
@@ -2388,7 +2391,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>2</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>2</v>
       </c>
@@ -2428,7 +2431,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>2</v>
       </c>
@@ -2448,7 +2451,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>2</v>
       </c>
@@ -2468,7 +2471,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>2</v>
       </c>
@@ -2488,7 +2491,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>2</v>
       </c>
@@ -2508,7 +2511,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>2</v>
       </c>
@@ -2528,7 +2531,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>2</v>
       </c>
@@ -2548,7 +2551,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>2</v>
       </c>
@@ -2568,7 +2571,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>2</v>
       </c>
@@ -2588,7 +2591,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>2</v>
       </c>
@@ -2608,7 +2611,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>2</v>
       </c>
@@ -2628,7 +2631,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>2</v>
       </c>
@@ -2648,7 +2651,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>2</v>
       </c>
@@ -2668,7 +2671,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>2</v>
       </c>
@@ -2688,7 +2691,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>2</v>
       </c>
@@ -2708,7 +2711,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>2</v>
       </c>
@@ -2728,7 +2731,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
@@ -2748,7 +2751,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>1</v>
       </c>
@@ -2768,7 +2771,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>1</v>
       </c>
@@ -2788,7 +2791,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>1</v>
       </c>
@@ -2808,7 +2811,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>1</v>
       </c>
@@ -2828,7 +2831,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>1</v>
       </c>
@@ -2848,7 +2851,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>1</v>
       </c>
@@ -2868,7 +2871,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>1</v>
       </c>
@@ -2888,7 +2891,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>1</v>
       </c>
@@ -2908,7 +2911,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>1</v>
       </c>
@@ -2928,7 +2931,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>1</v>
       </c>
@@ -2948,7 +2951,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>1</v>
       </c>
@@ -2968,7 +2971,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>1</v>
       </c>
@@ -2976,7 +2979,7 @@
         <v>28</v>
       </c>
       <c r="C92" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D92" t="s">
         <v>136</v>
@@ -2988,7 +2991,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>1</v>
       </c>
@@ -2996,10 +2999,10 @@
         <v>28</v>
       </c>
       <c r="C93" t="s">
+        <v>230</v>
+      </c>
+      <c r="D93" t="s">
         <v>137</v>
-      </c>
-      <c r="D93" t="s">
-        <v>138</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>40</v>
@@ -3008,7 +3011,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>1</v>
       </c>
@@ -3016,10 +3019,10 @@
         <v>28</v>
       </c>
       <c r="C94" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D94" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>40</v>
@@ -3028,7 +3031,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>1</v>
       </c>
@@ -3036,10 +3039,10 @@
         <v>28</v>
       </c>
       <c r="C95" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D95" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>40</v>
@@ -3048,7 +3051,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>1</v>
       </c>
@@ -3056,10 +3059,10 @@
         <v>28</v>
       </c>
       <c r="C96" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D96" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>40</v>
@@ -3068,7 +3071,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>1</v>
       </c>
@@ -3076,10 +3079,10 @@
         <v>28</v>
       </c>
       <c r="C97" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D97" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>40</v>
@@ -3088,7 +3091,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>1</v>
       </c>
@@ -3096,10 +3099,10 @@
         <v>28</v>
       </c>
       <c r="C98" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D98" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>40</v>
@@ -3108,7 +3111,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>1</v>
       </c>
@@ -3116,10 +3119,10 @@
         <v>28</v>
       </c>
       <c r="C99" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D99" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>40</v>
@@ -3128,7 +3131,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>1</v>
       </c>
@@ -3136,10 +3139,10 @@
         <v>28</v>
       </c>
       <c r="C100" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D100" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>40</v>
@@ -3148,7 +3151,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>1</v>
       </c>
@@ -3156,10 +3159,10 @@
         <v>28</v>
       </c>
       <c r="C101" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D101" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>40</v>
@@ -3168,7 +3171,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>1</v>
       </c>
@@ -3176,10 +3179,10 @@
         <v>28</v>
       </c>
       <c r="C102" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D102" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>40</v>
@@ -3188,7 +3191,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>1</v>
       </c>
@@ -3196,10 +3199,10 @@
         <v>28</v>
       </c>
       <c r="C103" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D103" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>40</v>
@@ -3208,7 +3211,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>1</v>
       </c>
@@ -3216,10 +3219,10 @@
         <v>28</v>
       </c>
       <c r="C104" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="D104" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>40</v>
@@ -3228,7 +3231,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>42</v>
       </c>
@@ -3236,10 +3239,10 @@
         <v>28</v>
       </c>
       <c r="C105" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="D105" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>41</v>
@@ -3248,7 +3251,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>42</v>
       </c>
@@ -3256,10 +3259,10 @@
         <v>28</v>
       </c>
       <c r="C106" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="D106" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>41</v>
@@ -3268,7 +3271,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>42</v>
       </c>
@@ -3276,10 +3279,10 @@
         <v>28</v>
       </c>
       <c r="C107" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="D107" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>41</v>
@@ -3288,7 +3291,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>42</v>
       </c>
@@ -3296,10 +3299,10 @@
         <v>28</v>
       </c>
       <c r="C108" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="D108" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E108" s="4" t="s">
         <v>41</v>
@@ -3308,7 +3311,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>42</v>
       </c>
@@ -3316,10 +3319,10 @@
         <v>28</v>
       </c>
       <c r="C109" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="D109" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>41</v>
@@ -3328,7 +3331,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>42</v>
       </c>
@@ -3339,7 +3342,7 @@
         <v>21</v>
       </c>
       <c r="D110" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E110" s="4" t="s">
         <v>41</v>
@@ -3348,7 +3351,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>42</v>
       </c>
@@ -3359,7 +3362,7 @@
         <v>21</v>
       </c>
       <c r="D111" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>41</v>
@@ -3368,7 +3371,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>42</v>
       </c>
@@ -3376,10 +3379,10 @@
         <v>28</v>
       </c>
       <c r="C112" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="D112" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E112" s="4" t="s">
         <v>41</v>
@@ -3388,7 +3391,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>42</v>
       </c>
@@ -3399,7 +3402,7 @@
         <v>21</v>
       </c>
       <c r="D113" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>41</v>
@@ -3408,7 +3411,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>42</v>
       </c>
@@ -3419,7 +3422,7 @@
         <v>21</v>
       </c>
       <c r="D114" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>41</v>
@@ -3428,7 +3431,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>42</v>
       </c>
@@ -3439,7 +3442,7 @@
         <v>21</v>
       </c>
       <c r="D115" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E115" s="4" t="s">
         <v>41</v>
@@ -3448,7 +3451,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>42</v>
       </c>
@@ -3459,7 +3462,7 @@
         <v>21</v>
       </c>
       <c r="D116" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E116" s="4" t="s">
         <v>41</v>
@@ -3468,7 +3471,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>42</v>
       </c>
@@ -3479,7 +3482,7 @@
         <v>21</v>
       </c>
       <c r="D117" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>41</v>
@@ -3488,7 +3491,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>42</v>
       </c>
@@ -3499,7 +3502,7 @@
         <v>21</v>
       </c>
       <c r="D118" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E118" s="4" t="s">
         <v>41</v>
@@ -3508,7 +3511,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>42</v>
       </c>
@@ -3519,7 +3522,7 @@
         <v>21</v>
       </c>
       <c r="D119" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E119" s="4" t="s">
         <v>41</v>
@@ -3528,7 +3531,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>42</v>
       </c>
@@ -3539,7 +3542,7 @@
         <v>21</v>
       </c>
       <c r="D120" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E120" s="4" t="s">
         <v>41</v>
@@ -3548,7 +3551,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>3</v>
       </c>
@@ -3559,16 +3562,16 @@
         <v>4</v>
       </c>
       <c r="D121" t="s">
-        <v>166</v>
-      </c>
-      <c r="E121" t="s">
+        <v>165</v>
+      </c>
+      <c r="E121" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F121" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>3</v>
       </c>
@@ -3579,16 +3582,16 @@
         <v>4</v>
       </c>
       <c r="D122" t="s">
-        <v>167</v>
-      </c>
-      <c r="E122" t="s">
+        <v>166</v>
+      </c>
+      <c r="E122" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F122" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>3</v>
       </c>
@@ -3599,16 +3602,16 @@
         <v>4</v>
       </c>
       <c r="D123" t="s">
-        <v>168</v>
-      </c>
-      <c r="E123" t="s">
+        <v>167</v>
+      </c>
+      <c r="E123" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F123" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>3</v>
       </c>
@@ -3619,16 +3622,16 @@
         <v>4</v>
       </c>
       <c r="D124" t="s">
-        <v>169</v>
-      </c>
-      <c r="E124" t="s">
+        <v>168</v>
+      </c>
+      <c r="E124" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F124" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>3</v>
       </c>
@@ -3639,16 +3642,16 @@
         <v>4</v>
       </c>
       <c r="D125" t="s">
-        <v>170</v>
-      </c>
-      <c r="E125" t="s">
+        <v>169</v>
+      </c>
+      <c r="E125" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F125" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>3</v>
       </c>
@@ -3659,16 +3662,16 @@
         <v>8</v>
       </c>
       <c r="D126" t="s">
-        <v>171</v>
-      </c>
-      <c r="E126" t="s">
+        <v>170</v>
+      </c>
+      <c r="E126" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F126" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>3</v>
       </c>
@@ -3679,16 +3682,16 @@
         <v>8</v>
       </c>
       <c r="D127" t="s">
-        <v>172</v>
-      </c>
-      <c r="E127" t="s">
+        <v>171</v>
+      </c>
+      <c r="E127" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F127" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>3</v>
       </c>
@@ -3699,16 +3702,16 @@
         <v>8</v>
       </c>
       <c r="D128" t="s">
-        <v>173</v>
-      </c>
-      <c r="E128" t="s">
+        <v>172</v>
+      </c>
+      <c r="E128" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F128" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>3</v>
       </c>
@@ -3719,16 +3722,16 @@
         <v>8</v>
       </c>
       <c r="D129" t="s">
-        <v>174</v>
-      </c>
-      <c r="E129" t="s">
+        <v>173</v>
+      </c>
+      <c r="E129" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F129" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>3</v>
       </c>
@@ -3739,16 +3742,16 @@
         <v>8</v>
       </c>
       <c r="D130" t="s">
-        <v>175</v>
-      </c>
-      <c r="E130" t="s">
+        <v>174</v>
+      </c>
+      <c r="E130" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F130" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>3</v>
       </c>
@@ -3759,16 +3762,16 @@
         <v>8</v>
       </c>
       <c r="D131" t="s">
-        <v>176</v>
-      </c>
-      <c r="E131" t="s">
+        <v>175</v>
+      </c>
+      <c r="E131" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F131" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>3</v>
       </c>
@@ -3779,16 +3782,16 @@
         <v>8</v>
       </c>
       <c r="D132" t="s">
-        <v>177</v>
-      </c>
-      <c r="E132" t="s">
+        <v>176</v>
+      </c>
+      <c r="E132" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F132" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>3</v>
       </c>
@@ -3799,16 +3802,16 @@
         <v>8</v>
       </c>
       <c r="D133" t="s">
-        <v>178</v>
-      </c>
-      <c r="E133" t="s">
+        <v>177</v>
+      </c>
+      <c r="E133" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F133" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>3</v>
       </c>
@@ -3819,16 +3822,16 @@
         <v>8</v>
       </c>
       <c r="D134" t="s">
-        <v>179</v>
-      </c>
-      <c r="E134" t="s">
+        <v>178</v>
+      </c>
+      <c r="E134" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F134" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>3</v>
       </c>
@@ -3839,16 +3842,16 @@
         <v>8</v>
       </c>
       <c r="D135" t="s">
-        <v>180</v>
-      </c>
-      <c r="E135" t="s">
+        <v>179</v>
+      </c>
+      <c r="E135" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F135" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>3</v>
       </c>
@@ -3859,16 +3862,16 @@
         <v>8</v>
       </c>
       <c r="D136" t="s">
-        <v>181</v>
-      </c>
-      <c r="E136" t="s">
+        <v>180</v>
+      </c>
+      <c r="E136" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F136" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>3</v>
       </c>
@@ -3879,16 +3882,16 @@
         <v>8</v>
       </c>
       <c r="D137" t="s">
-        <v>182</v>
-      </c>
-      <c r="E137" t="s">
+        <v>181</v>
+      </c>
+      <c r="E137" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F137" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>1</v>
       </c>
@@ -3899,16 +3902,16 @@
         <v>18</v>
       </c>
       <c r="D138" t="s">
-        <v>183</v>
-      </c>
-      <c r="E138" t="s">
+        <v>182</v>
+      </c>
+      <c r="E138" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F138" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>1</v>
       </c>
@@ -3919,16 +3922,16 @@
         <v>18</v>
       </c>
       <c r="D139" t="s">
-        <v>184</v>
-      </c>
-      <c r="E139" t="s">
+        <v>183</v>
+      </c>
+      <c r="E139" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F139" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>1</v>
       </c>
@@ -3939,16 +3942,16 @@
         <v>18</v>
       </c>
       <c r="D140" t="s">
-        <v>185</v>
-      </c>
-      <c r="E140" t="s">
+        <v>184</v>
+      </c>
+      <c r="E140" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F140" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>1</v>
       </c>
@@ -3959,16 +3962,16 @@
         <v>18</v>
       </c>
       <c r="D141" t="s">
-        <v>186</v>
-      </c>
-      <c r="E141" t="s">
+        <v>185</v>
+      </c>
+      <c r="E141" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F141" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>1</v>
       </c>
@@ -3979,16 +3982,16 @@
         <v>18</v>
       </c>
       <c r="D142" t="s">
-        <v>187</v>
-      </c>
-      <c r="E142" t="s">
+        <v>186</v>
+      </c>
+      <c r="E142" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F142" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>1</v>
       </c>
@@ -3999,16 +4002,16 @@
         <v>18</v>
       </c>
       <c r="D143" t="s">
-        <v>188</v>
-      </c>
-      <c r="E143" t="s">
+        <v>187</v>
+      </c>
+      <c r="E143" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F143" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>1</v>
       </c>
@@ -4019,16 +4022,16 @@
         <v>18</v>
       </c>
       <c r="D144" t="s">
-        <v>189</v>
-      </c>
-      <c r="E144" t="s">
+        <v>188</v>
+      </c>
+      <c r="E144" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F144" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>1</v>
       </c>
@@ -4039,16 +4042,16 @@
         <v>18</v>
       </c>
       <c r="D145" t="s">
-        <v>190</v>
-      </c>
-      <c r="E145" t="s">
+        <v>189</v>
+      </c>
+      <c r="E145" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F145" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>1</v>
       </c>
@@ -4059,16 +4062,16 @@
         <v>18</v>
       </c>
       <c r="D146" t="s">
-        <v>191</v>
-      </c>
-      <c r="E146" t="s">
+        <v>190</v>
+      </c>
+      <c r="E146" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F146" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>2</v>
       </c>
@@ -4079,16 +4082,16 @@
         <v>5</v>
       </c>
       <c r="D147" t="s">
-        <v>192</v>
-      </c>
-      <c r="E147" t="s">
+        <v>191</v>
+      </c>
+      <c r="E147" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F147" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>2</v>
       </c>
@@ -4099,7 +4102,7 @@
         <v>5</v>
       </c>
       <c r="D148" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E148" s="4" t="s">
         <v>46</v>
@@ -4108,7 +4111,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>2</v>
       </c>
@@ -4119,16 +4122,16 @@
         <v>5</v>
       </c>
       <c r="D149" t="s">
-        <v>194</v>
-      </c>
-      <c r="E149" t="s">
+        <v>193</v>
+      </c>
+      <c r="E149" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F149" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>2</v>
       </c>
@@ -4139,7 +4142,7 @@
         <v>5</v>
       </c>
       <c r="D150" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E150" s="4" t="s">
         <v>46</v>
@@ -4148,7 +4151,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>2</v>
       </c>
@@ -4159,16 +4162,16 @@
         <v>5</v>
       </c>
       <c r="D151" t="s">
-        <v>196</v>
-      </c>
-      <c r="E151" t="s">
+        <v>195</v>
+      </c>
+      <c r="E151" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F151" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>22</v>
       </c>
@@ -4179,16 +4182,16 @@
         <v>19</v>
       </c>
       <c r="D152" t="s">
-        <v>197</v>
-      </c>
-      <c r="E152" t="s">
+        <v>196</v>
+      </c>
+      <c r="E152" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F152" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>22</v>
       </c>
@@ -4199,16 +4202,16 @@
         <v>19</v>
       </c>
       <c r="D153" t="s">
-        <v>198</v>
-      </c>
-      <c r="E153" t="s">
+        <v>197</v>
+      </c>
+      <c r="E153" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F153" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>22</v>
       </c>
@@ -4219,16 +4222,16 @@
         <v>19</v>
       </c>
       <c r="D154" t="s">
-        <v>199</v>
-      </c>
-      <c r="E154" t="s">
+        <v>198</v>
+      </c>
+      <c r="E154" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F154" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>22</v>
       </c>
@@ -4239,16 +4242,16 @@
         <v>19</v>
       </c>
       <c r="D155" t="s">
-        <v>200</v>
-      </c>
-      <c r="E155" t="s">
+        <v>199</v>
+      </c>
+      <c r="E155" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F155" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>22</v>
       </c>
@@ -4259,16 +4262,16 @@
         <v>19</v>
       </c>
       <c r="D156" t="s">
-        <v>201</v>
-      </c>
-      <c r="E156" t="s">
+        <v>200</v>
+      </c>
+      <c r="E156" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F156" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>22</v>
       </c>
@@ -4279,16 +4282,16 @@
         <v>19</v>
       </c>
       <c r="D157" t="s">
-        <v>202</v>
-      </c>
-      <c r="E157" t="s">
+        <v>201</v>
+      </c>
+      <c r="E157" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F157" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>22</v>
       </c>
@@ -4299,16 +4302,16 @@
         <v>19</v>
       </c>
       <c r="D158" t="s">
-        <v>203</v>
-      </c>
-      <c r="E158" t="s">
+        <v>202</v>
+      </c>
+      <c r="E158" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F158" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>22</v>
       </c>
@@ -4319,16 +4322,16 @@
         <v>19</v>
       </c>
       <c r="D159" t="s">
-        <v>204</v>
-      </c>
-      <c r="E159" t="s">
+        <v>203</v>
+      </c>
+      <c r="E159" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F159" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>22</v>
       </c>
@@ -4339,16 +4342,16 @@
         <v>19</v>
       </c>
       <c r="D160" t="s">
-        <v>205</v>
-      </c>
-      <c r="E160" t="s">
+        <v>204</v>
+      </c>
+      <c r="E160" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F160" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>22</v>
       </c>
@@ -4359,16 +4362,16 @@
         <v>19</v>
       </c>
       <c r="D161" t="s">
-        <v>206</v>
-      </c>
-      <c r="E161" t="s">
+        <v>205</v>
+      </c>
+      <c r="E161" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F161" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>22</v>
       </c>
@@ -4379,16 +4382,16 @@
         <v>19</v>
       </c>
       <c r="D162" t="s">
-        <v>207</v>
-      </c>
-      <c r="E162" t="s">
+        <v>206</v>
+      </c>
+      <c r="E162" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F162" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>22</v>
       </c>
@@ -4399,16 +4402,16 @@
         <v>19</v>
       </c>
       <c r="D163" t="s">
-        <v>208</v>
-      </c>
-      <c r="E163" t="s">
+        <v>207</v>
+      </c>
+      <c r="E163" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F163" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>22</v>
       </c>
@@ -4419,16 +4422,16 @@
         <v>19</v>
       </c>
       <c r="D164" t="s">
-        <v>209</v>
-      </c>
-      <c r="E164" t="s">
+        <v>208</v>
+      </c>
+      <c r="E164" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F164" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>22</v>
       </c>
@@ -4439,16 +4442,16 @@
         <v>19</v>
       </c>
       <c r="D165" t="s">
-        <v>210</v>
-      </c>
-      <c r="E165" t="s">
+        <v>209</v>
+      </c>
+      <c r="E165" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F165" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>22</v>
       </c>
@@ -4459,16 +4462,16 @@
         <v>20</v>
       </c>
       <c r="D166" t="s">
-        <v>211</v>
-      </c>
-      <c r="E166" t="s">
+        <v>210</v>
+      </c>
+      <c r="E166" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F166" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>22</v>
       </c>
@@ -4479,16 +4482,16 @@
         <v>20</v>
       </c>
       <c r="D167" t="s">
-        <v>212</v>
-      </c>
-      <c r="E167" t="s">
+        <v>211</v>
+      </c>
+      <c r="E167" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F167" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>22</v>
       </c>
@@ -4499,16 +4502,16 @@
         <v>20</v>
       </c>
       <c r="D168" t="s">
-        <v>213</v>
-      </c>
-      <c r="E168" t="s">
+        <v>212</v>
+      </c>
+      <c r="E168" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F168" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>22</v>
       </c>
@@ -4519,16 +4522,16 @@
         <v>20</v>
       </c>
       <c r="D169" t="s">
-        <v>214</v>
-      </c>
-      <c r="E169" t="s">
+        <v>213</v>
+      </c>
+      <c r="E169" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F169" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>22</v>
       </c>
@@ -4539,16 +4542,16 @@
         <v>20</v>
       </c>
       <c r="D170" t="s">
-        <v>215</v>
-      </c>
-      <c r="E170" t="s">
+        <v>214</v>
+      </c>
+      <c r="E170" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F170" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>22</v>
       </c>
@@ -4559,16 +4562,16 @@
         <v>20</v>
       </c>
       <c r="D171" t="s">
-        <v>216</v>
-      </c>
-      <c r="E171" t="s">
+        <v>215</v>
+      </c>
+      <c r="E171" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F171" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>22</v>
       </c>
@@ -4579,16 +4582,16 @@
         <v>20</v>
       </c>
       <c r="D172" t="s">
-        <v>217</v>
-      </c>
-      <c r="E172" t="s">
+        <v>216</v>
+      </c>
+      <c r="E172" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F172" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>22</v>
       </c>
@@ -4599,16 +4602,16 @@
         <v>20</v>
       </c>
       <c r="D173" t="s">
-        <v>218</v>
-      </c>
-      <c r="E173" t="s">
+        <v>217</v>
+      </c>
+      <c r="E173" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F173" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>22</v>
       </c>
@@ -4619,16 +4622,16 @@
         <v>20</v>
       </c>
       <c r="D174" t="s">
-        <v>219</v>
-      </c>
-      <c r="E174" t="s">
+        <v>218</v>
+      </c>
+      <c r="E174" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F174" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>3</v>
       </c>
@@ -4639,7 +4642,7 @@
         <v>14</v>
       </c>
       <c r="D175" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E175" s="4" t="s">
         <v>36</v>
@@ -4648,7 +4651,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>3</v>
       </c>
@@ -4659,7 +4662,7 @@
         <v>14</v>
       </c>
       <c r="D176" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E176" s="4" t="s">
         <v>36</v>
@@ -4668,7 +4671,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>3</v>
       </c>
@@ -4679,7 +4682,7 @@
         <v>14</v>
       </c>
       <c r="D177" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E177" s="4" t="s">
         <v>36</v>
@@ -4688,7 +4691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>3</v>
       </c>
@@ -4699,7 +4702,7 @@
         <v>14</v>
       </c>
       <c r="D178" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E178" s="4" t="s">
         <v>36</v>
@@ -4708,7 +4711,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>3</v>
       </c>
@@ -4719,7 +4722,7 @@
         <v>14</v>
       </c>
       <c r="D179" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E179" s="4" t="s">
         <v>36</v>
@@ -4728,7 +4731,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>3</v>
       </c>
@@ -4739,7 +4742,7 @@
         <v>14</v>
       </c>
       <c r="D180" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E180" s="4" t="s">
         <v>36</v>
@@ -4748,7 +4751,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>42</v>
       </c>
@@ -4756,19 +4759,19 @@
         <v>28</v>
       </c>
       <c r="C181" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="D181" t="s">
-        <v>226</v>
-      </c>
-      <c r="E181" t="s">
+        <v>225</v>
+      </c>
+      <c r="E181" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F181" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>42</v>
       </c>
@@ -4776,19 +4779,19 @@
         <v>28</v>
       </c>
       <c r="C182" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="D182" t="s">
-        <v>227</v>
-      </c>
-      <c r="E182" t="s">
+        <v>226</v>
+      </c>
+      <c r="E182" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F182" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>42</v>
       </c>
@@ -4796,12 +4799,12 @@
         <v>28</v>
       </c>
       <c r="C183" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="E183" t="s">
+        <v>227</v>
+      </c>
+      <c r="E183" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F183" t="s">
@@ -4812,7 +4815,7 @@
   <autoFilter ref="A1:F183" xr:uid="{662A6874-D8A2-496A-8EEF-D3372C3E2EBA}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Jariiban"/>
+        <filter val="Galkacyo"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
rural and urban consolidation
this is done before merging with danwadaag
</commit_message>
<xml_diff>
--- a/docs/ewea/ewea communities districts and fms.xlsx
+++ b/docs/ewea/ewea communities districts and fms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs Developement\rstudio\Testing\core\docs\ewea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC878CE9-1DC1-4CF0-80DE-0907047C75FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998F7BC8-C101-4EF7-9942-F4826DD1262D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0052D8CE-578C-4384-ABBC-B6D3FDE38954}"/>
   </bookViews>
@@ -804,7 +804,18 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{34D20D2E-F27D-4C2D-AD01-9BEBE98DF909}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1134,11 +1145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662A6874-D8A2-496A-8EEF-D3372C3E2EBA}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F183"/>
+  <dimension ref="A1:F188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1181,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1191,7 +1201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1211,7 +1221,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1231,7 +1241,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1251,7 +1261,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1271,7 +1281,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1291,7 +1301,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1311,7 +1321,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1331,7 +1341,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1351,7 +1361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1371,7 +1381,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1391,7 +1401,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1411,7 +1421,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -1431,7 +1441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1451,7 +1461,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1471,7 +1481,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1491,7 +1501,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -1511,7 +1521,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1531,7 +1541,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -1551,7 +1561,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -1571,7 +1581,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -1591,7 +1601,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1611,7 +1621,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -1631,7 +1641,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -1651,7 +1661,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1671,7 +1681,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1691,7 +1701,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -1711,7 +1721,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -1731,7 +1741,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1751,7 +1761,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -1771,7 +1781,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
@@ -1791,7 +1801,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
@@ -1811,7 +1821,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
@@ -1831,7 +1841,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -1851,7 +1861,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
@@ -1871,7 +1881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -1891,7 +1901,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
@@ -1911,7 +1921,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -1931,7 +1941,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -1951,7 +1961,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
@@ -1971,7 +1981,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
@@ -1991,7 +2001,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
@@ -2011,7 +2021,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
@@ -2031,7 +2041,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -2051,7 +2061,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
@@ -2071,7 +2081,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
@@ -2091,7 +2101,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
@@ -2111,7 +2121,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -2131,7 +2141,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -2151,7 +2161,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
@@ -2171,7 +2181,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>2</v>
       </c>
@@ -2191,7 +2201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>2</v>
       </c>
@@ -2211,7 +2221,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>2</v>
       </c>
@@ -2231,7 +2241,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>2</v>
       </c>
@@ -2251,7 +2261,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>2</v>
       </c>
@@ -2271,7 +2281,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>2</v>
       </c>
@@ -2291,7 +2301,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>2</v>
       </c>
@@ -2311,7 +2321,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>2</v>
       </c>
@@ -2331,7 +2341,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>2</v>
       </c>
@@ -2351,7 +2361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
@@ -2371,7 +2381,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>2</v>
       </c>
@@ -2391,7 +2401,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>2</v>
       </c>
@@ -2411,7 +2421,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>2</v>
       </c>
@@ -2431,7 +2441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>2</v>
       </c>
@@ -2451,7 +2461,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>2</v>
       </c>
@@ -2471,7 +2481,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>2</v>
       </c>
@@ -2491,7 +2501,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>2</v>
       </c>
@@ -2511,7 +2521,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>2</v>
       </c>
@@ -2531,7 +2541,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>2</v>
       </c>
@@ -2551,7 +2561,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>2</v>
       </c>
@@ -2571,7 +2581,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>2</v>
       </c>
@@ -2591,7 +2601,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>2</v>
       </c>
@@ -2611,7 +2621,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>2</v>
       </c>
@@ -2631,7 +2641,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>2</v>
       </c>
@@ -2651,7 +2661,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>2</v>
       </c>
@@ -2671,7 +2681,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>2</v>
       </c>
@@ -2691,7 +2701,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>2</v>
       </c>
@@ -2711,7 +2721,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>2</v>
       </c>
@@ -2731,7 +2741,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
@@ -2751,7 +2761,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>1</v>
       </c>
@@ -2771,7 +2781,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>1</v>
       </c>
@@ -2791,7 +2801,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>1</v>
       </c>
@@ -2811,7 +2821,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>1</v>
       </c>
@@ -2831,7 +2841,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>1</v>
       </c>
@@ -2851,7 +2861,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>1</v>
       </c>
@@ -2871,7 +2881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>1</v>
       </c>
@@ -2891,7 +2901,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>1</v>
       </c>
@@ -2911,7 +2921,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>1</v>
       </c>
@@ -2931,7 +2941,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>1</v>
       </c>
@@ -2951,7 +2961,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>1</v>
       </c>
@@ -3331,7 +3341,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>42</v>
       </c>
@@ -3351,7 +3361,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>42</v>
       </c>
@@ -3391,7 +3401,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>42</v>
       </c>
@@ -3411,7 +3421,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>42</v>
       </c>
@@ -3431,7 +3441,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>42</v>
       </c>
@@ -3451,7 +3461,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>42</v>
       </c>
@@ -3471,7 +3481,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>42</v>
       </c>
@@ -3491,7 +3501,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>42</v>
       </c>
@@ -3511,7 +3521,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>42</v>
       </c>
@@ -3531,7 +3541,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>42</v>
       </c>
@@ -3551,7 +3561,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>3</v>
       </c>
@@ -3571,7 +3581,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>3</v>
       </c>
@@ -3591,7 +3601,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>3</v>
       </c>
@@ -3611,7 +3621,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>3</v>
       </c>
@@ -3631,7 +3641,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>3</v>
       </c>
@@ -3651,7 +3661,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>3</v>
       </c>
@@ -3671,7 +3681,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>3</v>
       </c>
@@ -3691,7 +3701,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>3</v>
       </c>
@@ -3711,7 +3721,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>3</v>
       </c>
@@ -3731,7 +3741,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>3</v>
       </c>
@@ -3751,7 +3761,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>3</v>
       </c>
@@ -3771,7 +3781,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>3</v>
       </c>
@@ -3791,7 +3801,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>3</v>
       </c>
@@ -3811,7 +3821,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>3</v>
       </c>
@@ -3831,7 +3841,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>3</v>
       </c>
@@ -3851,7 +3861,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>3</v>
       </c>
@@ -3871,7 +3881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>3</v>
       </c>
@@ -3891,7 +3901,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>1</v>
       </c>
@@ -3911,7 +3921,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>1</v>
       </c>
@@ -3931,7 +3941,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>1</v>
       </c>
@@ -3951,7 +3961,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>1</v>
       </c>
@@ -3971,7 +3981,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>1</v>
       </c>
@@ -3991,7 +4001,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>1</v>
       </c>
@@ -4011,7 +4021,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>1</v>
       </c>
@@ -4031,7 +4041,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>1</v>
       </c>
@@ -4051,7 +4061,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>1</v>
       </c>
@@ -4071,7 +4081,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>2</v>
       </c>
@@ -4091,7 +4101,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>2</v>
       </c>
@@ -4111,7 +4121,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>2</v>
       </c>
@@ -4131,7 +4141,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>2</v>
       </c>
@@ -4151,7 +4161,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>2</v>
       </c>
@@ -4171,7 +4181,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>22</v>
       </c>
@@ -4191,7 +4201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>22</v>
       </c>
@@ -4211,7 +4221,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>22</v>
       </c>
@@ -4231,7 +4241,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>22</v>
       </c>
@@ -4251,7 +4261,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>22</v>
       </c>
@@ -4271,7 +4281,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>22</v>
       </c>
@@ -4291,7 +4301,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>22</v>
       </c>
@@ -4311,7 +4321,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>22</v>
       </c>
@@ -4331,7 +4341,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>22</v>
       </c>
@@ -4351,7 +4361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>22</v>
       </c>
@@ -4371,7 +4381,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>22</v>
       </c>
@@ -4391,7 +4401,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>22</v>
       </c>
@@ -4411,7 +4421,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>22</v>
       </c>
@@ -4431,7 +4441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>22</v>
       </c>
@@ -4451,7 +4461,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>22</v>
       </c>
@@ -4471,7 +4481,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>22</v>
       </c>
@@ -4491,7 +4501,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>22</v>
       </c>
@@ -4511,7 +4521,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>22</v>
       </c>
@@ -4531,7 +4541,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>22</v>
       </c>
@@ -4551,7 +4561,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>22</v>
       </c>
@@ -4571,7 +4581,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>22</v>
       </c>
@@ -4591,7 +4601,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>22</v>
       </c>
@@ -4611,7 +4621,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>22</v>
       </c>
@@ -4631,7 +4641,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>3</v>
       </c>
@@ -4651,7 +4661,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>3</v>
       </c>
@@ -4671,7 +4681,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>3</v>
       </c>
@@ -4691,7 +4701,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>3</v>
       </c>
@@ -4711,7 +4721,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>3</v>
       </c>
@@ -4731,7 +4741,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>3</v>
       </c>
@@ -4811,14 +4821,41 @@
         <v>45</v>
       </c>
     </row>
+    <row r="184" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A184" s="1"/>
+      <c r="B184" s="2"/>
+      <c r="D184" s="3"/>
+      <c r="E184" s="4"/>
+    </row>
+    <row r="185" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A185" s="1"/>
+      <c r="B185" s="2"/>
+      <c r="D185" s="3"/>
+      <c r="E185" s="4"/>
+    </row>
+    <row r="186" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A186" s="1"/>
+      <c r="B186" s="2"/>
+      <c r="D186" s="3"/>
+      <c r="E186" s="4"/>
+    </row>
+    <row r="187" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A187" s="1"/>
+      <c r="B187" s="2"/>
+      <c r="D187" s="3"/>
+      <c r="E187" s="4"/>
+    </row>
+    <row r="188" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A188" s="1"/>
+      <c r="B188" s="2"/>
+      <c r="D188" s="3"/>
+      <c r="E188" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F183" xr:uid="{662A6874-D8A2-496A-8EEF-D3372C3E2EBA}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Galkacyo"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F183" xr:uid="{662A6874-D8A2-496A-8EEF-D3372C3E2EBA}"/>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated districts and thresholds with danwadaag areas
</commit_message>
<xml_diff>
--- a/docs/ewea/ewea communities districts and fms.xlsx
+++ b/docs/ewea/ewea communities districts and fms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs Developement\rstudio\Testing\core\docs\ewea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998F7BC8-C101-4EF7-9942-F4826DD1262D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9545E73-6FAC-4C60-9564-1E5C86D39451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0052D8CE-578C-4384-ABBC-B6D3FDE38954}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="253">
   <si>
     <t>FMS</t>
   </si>
@@ -732,6 +732,72 @@
   </si>
   <si>
     <t>Galkacyo-South</t>
+  </si>
+  <si>
+    <t>baidoa__ca1</t>
+  </si>
+  <si>
+    <t>baidoa__ca3</t>
+  </si>
+  <si>
+    <t>baidoa__ca4</t>
+  </si>
+  <si>
+    <t>baidoa__ca11</t>
+  </si>
+  <si>
+    <t>IOM</t>
+  </si>
+  <si>
+    <t>Shida</t>
+  </si>
+  <si>
+    <t>Wadajir</t>
+  </si>
+  <si>
+    <t>Fanole</t>
+  </si>
+  <si>
+    <t>Calanley</t>
+  </si>
+  <si>
+    <t>Luglow</t>
+  </si>
+  <si>
+    <t>Dolow</t>
+  </si>
+  <si>
+    <t>Qurdubey</t>
+  </si>
+  <si>
+    <t>Kaxaarey</t>
+  </si>
+  <si>
+    <t>Berdale</t>
+  </si>
+  <si>
+    <t>Oktober</t>
+  </si>
+  <si>
+    <t>x_keskey</t>
+  </si>
+  <si>
+    <t>Banadir</t>
+  </si>
+  <si>
+    <t>Mogadishu</t>
+  </si>
+  <si>
+    <t>Daynile</t>
+  </si>
+  <si>
+    <t>Kahda</t>
+  </si>
+  <si>
+    <t>ca19</t>
+  </si>
+  <si>
+    <t>ca6</t>
   </si>
 </sst>
 </file>
@@ -749,6 +815,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -770,12 +837,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -791,7 +864,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -799,6 +872,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1145,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662A6874-D8A2-496A-8EEF-D3372C3E2EBA}">
-  <dimension ref="A1:F188"/>
+  <dimension ref="A1:F198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="F190" sqref="F190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4821,35 +4901,305 @@
         <v>45</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A184" s="1"/>
-      <c r="B184" s="2"/>
-      <c r="D184" s="3"/>
-      <c r="E184" s="4"/>
+    <row r="184" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A184" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C184" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D184" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="E184" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F184" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="185" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A185" s="1"/>
-      <c r="B185" s="2"/>
-      <c r="D185" s="3"/>
-      <c r="E185" s="4"/>
+      <c r="A185" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C185" t="s">
+        <v>5</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E185" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F185" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="186" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="1"/>
-      <c r="B186" s="2"/>
-      <c r="D186" s="3"/>
-      <c r="E186" s="4"/>
+      <c r="A186" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C186" t="s">
+        <v>5</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E186" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F186" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="187" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A187" s="1"/>
-      <c r="B187" s="2"/>
-      <c r="D187" s="3"/>
-      <c r="E187" s="4"/>
+      <c r="A187" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C187" t="s">
+        <v>5</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E187" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F187" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="188" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A188" s="1"/>
-      <c r="B188" s="2"/>
-      <c r="D188" s="3"/>
-      <c r="E188" s="4"/>
+      <c r="A188" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C188" t="s">
+        <v>7</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E188" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F188" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C189" t="s">
+        <v>7</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E189" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F189" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C190" t="s">
+        <v>8</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E190" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F190" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C191" t="s">
+        <v>8</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E191" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F191" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C192" t="s">
+        <v>8</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E192" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F192" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C193" t="s">
+        <v>241</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E193" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F193" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C194" t="s">
+        <v>241</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E194" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F194" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C195" t="s">
+        <v>244</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E195" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F195" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C196" t="s">
+        <v>14</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E196" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F196" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C197" t="s">
+        <v>249</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E197" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F197" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C198" t="s">
+        <v>250</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E198" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F198" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F183" xr:uid="{662A6874-D8A2-496A-8EEF-D3372C3E2EBA}"/>

</xml_diff>